<commit_message>
chore: update output templates to newest versions
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\do.treas.gov\dfsres\isilon\Homeshare3\BerrocalF\XenProfile\Desktop\SLFRF P&amp;E Quarter 2 Bulk Files\UpdateTemplates.6.21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/42853_icf_com/Documents/Bulk Upload/Templates/9.8/July Project Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB500CE3-B6D0-4EFB-8B1A-1853A5379974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BB500CE3-B6D0-4EFB-8B1A-1853A5379974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E2F7F2-7D4F-4E8A-86CB-AD0668BC0434}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="90" windowWidth="29040" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -369,12 +369,6 @@
     <t>Number_People_Summer_Youth__c</t>
   </si>
   <si>
-    <t>Q2_2022_Obligations__c</t>
-  </si>
-  <si>
-    <t>Q2_2022_Expenditures__c</t>
-  </si>
-  <si>
     <t>The total dollar value of obligations for this project.  
 Currency field. 
 DO NOT include a "$" sign or commas "," when entering Amounts.</t>
@@ -457,6 +451,12 @@
   </si>
   <si>
     <t>Version: 2022.06.21</t>
+  </si>
+  <si>
+    <t>Q3_2022_Obligations__c</t>
+  </si>
+  <si>
+    <t>Q3_2022_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -621,51 +621,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -684,11 +667,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -922,18 +902,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FAA55-771D-4D64-A81A-E1231934DFE3}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53" style="2" customWidth="1"/>
     <col min="2" max="5" width="35.625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="35.5" style="4" customWidth="1"/>
-    <col min="8" max="15" width="35.625" style="2" customWidth="1"/>
-    <col min="16" max="17" width="35.625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="35.625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="35.5" style="2" customWidth="1"/>
+    <col min="8" max="18" width="35.625" style="2" customWidth="1"/>
     <col min="19" max="19" width="29" style="2" customWidth="1"/>
     <col min="20" max="23" width="25.125" style="2" customWidth="1"/>
     <col min="24" max="24" width="28.875" style="2" customWidth="1"/>
@@ -947,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -982,10 +960,10 @@
       <c r="AF1" s="1"/>
     </row>
     <row r="2" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1018,10 +996,10 @@
       <c r="AF2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="206.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1054,626 +1032,626 @@
       <c r="AF3" s="1"/>
     </row>
     <row r="4" spans="1:32" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>90</v>
+      <c r="G4" s="4" t="s">
+        <v>88</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>77</v>
+      <c r="K4" s="4" t="s">
+        <v>93</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>78</v>
+      <c r="L4" s="4" t="s">
+        <v>94</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Y4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="Z4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AA4" s="5" t="s">
+      <c r="AA4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" s="5" t="s">
+      <c r="AB4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AC4" s="7" t="s">
+      <c r="AC4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AD4" s="7" t="s">
+      <c r="AD4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AE4" s="7" t="s">
+      <c r="AE4" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AF4" s="1"/>
     </row>
     <row r="5" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="T5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="X5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AA5" s="7" t="s">
+      <c r="AA5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AB5" s="5" t="s">
+      <c r="AB5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AC5" s="7" t="s">
+      <c r="AC5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AD5" s="7" t="s">
+      <c r="AD5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AE5" s="7" t="s">
+      <c r="AE5" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AF5" s="1"/>
     </row>
     <row r="6" spans="1:32" ht="48.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>91</v>
+      <c r="G6" s="4" t="s">
+        <v>89</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="15" t="s">
+      <c r="U6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="W6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="X6" s="15" t="s">
+      <c r="X6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="Y6" s="15" t="s">
+      <c r="Y6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Z6" s="15" t="s">
+      <c r="Z6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AA6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AB6" s="15" t="s">
+      <c r="AB6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AC6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AD6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AE6" s="6" t="s">
         <v>73</v>
       </c>
       <c r="AF6" s="3"/>
     </row>
     <row r="7" spans="1:32" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>92</v>
+      <c r="F7" s="12" t="s">
+        <v>90</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>93</v>
+      <c r="G7" s="12" t="s">
+        <v>91</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>88</v>
+      <c r="H7" s="11" t="s">
+        <v>86</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="L7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="M7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="T7" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="M7" s="18" t="s">
-        <v>29</v>
+      <c r="U7" s="11" t="s">
+        <v>66</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>89</v>
+      <c r="V7" s="11" t="s">
+        <v>65</v>
       </c>
-      <c r="O7" s="17" t="s">
-        <v>68</v>
+      <c r="W7" s="11" t="s">
+        <v>66</v>
       </c>
-      <c r="P7" s="18" t="s">
-        <v>54</v>
+      <c r="X7" s="11" t="s">
+        <v>65</v>
       </c>
-      <c r="Q7" s="17" t="s">
-        <v>51</v>
+      <c r="Y7" s="11" t="s">
+        <v>66</v>
       </c>
-      <c r="R7" s="18" t="s">
-        <v>20</v>
+      <c r="Z7" s="11" t="s">
+        <v>65</v>
       </c>
-      <c r="S7" s="18" t="s">
+      <c r="AA7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE7" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="T7" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="U7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="V7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="W7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="X7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB7" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC7" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD7" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE7" s="17" t="s">
-        <v>85</v>
-      </c>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" s="12" customFormat="1" ht="43.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-    </row>
-    <row r="9" spans="1:32" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-    </row>
-    <row r="10" spans="1:32" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+    <row r="8" spans="1:32" ht="43.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+    </row>
+    <row r="9" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+    </row>
+    <row r="10" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-    </row>
-    <row r="11" spans="1:32" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+    </row>
+    <row r="11" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="11"/>
-    </row>
-    <row r="12" spans="1:32" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="1"/>
+    </row>
+    <row r="12" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="11"/>
-    </row>
-    <row r="13" spans="1:32" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="1"/>
+    </row>
+    <row r="13" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="14"/>
-    </row>
-    <row r="14" spans="1:32" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="3"/>
+    </row>
+    <row r="14" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="10"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="11"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="1"/>
     </row>
     <row r="15" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -35209,9 +35187,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -35432,27 +35413,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -35477,9 +35446,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore: update for jan 2023 output templates
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/42853_icf_com/Documents/Bulk Upload/Templates/9.8/July Project Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 4 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BB500CE3-B6D0-4EFB-8B1A-1853A5379974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E2F7F2-7D4F-4E8A-86CB-AD0668BC0434}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C15497B-6C8E-434C-9B6A-CDFB32373EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Version: 2022.06.21</t>
+    <t>Q4_2022_Obligations__c</t>
   </si>
   <si>
-    <t>Q3_2022_Obligations__c</t>
+    <t>Q4_2022_Expenditures__c</t>
   </si>
   <si>
-    <t>Q3_2022_Expenditures__c</t>
+    <t>Version: 2022.12.13</t>
   </si>
 </sst>
 </file>
@@ -902,9 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FAA55-771D-4D64-A81A-E1231934DFE3}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -925,7 +923,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1063,10 +1061,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>30</v>
@@ -35187,6 +35185,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -35195,7 +35199,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35412,13 +35416,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -35426,7 +35441,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35443,21 +35458,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Prod release Jan 17 2023 (#822)
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/42853_icf_com/Documents/Bulk Upload/Templates/9.8/July Project Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 4 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BB500CE3-B6D0-4EFB-8B1A-1853A5379974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E2F7F2-7D4F-4E8A-86CB-AD0668BC0434}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C15497B-6C8E-434C-9B6A-CDFB32373EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Version: 2022.06.21</t>
+    <t>Q4_2022_Obligations__c</t>
   </si>
   <si>
-    <t>Q3_2022_Obligations__c</t>
+    <t>Q4_2022_Expenditures__c</t>
   </si>
   <si>
-    <t>Q3_2022_Expenditures__c</t>
+    <t>Version: 2022.12.13</t>
   </si>
 </sst>
 </file>
@@ -902,9 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FAA55-771D-4D64-A81A-E1231934DFE3}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -925,7 +923,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1063,10 +1061,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>30</v>
@@ -35187,6 +35185,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -35195,7 +35199,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35412,13 +35416,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -35426,7 +35441,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35443,21 +35458,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: update q1 2023 output templates (#1273)
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 4 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pridgenc\Downloads\SLFRFBulkUploadTemplates\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C15497B-6C8E-434C-9B6A-CDFB32373EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16356CFA-53BD-4FBD-B03E-C69286943FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="4845" windowWidth="25815" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Q4_2022_Obligations__c</t>
+    <t>Q1_2023_Obligations__c</t>
   </si>
   <si>
-    <t>Q4_2022_Expenditures__c</t>
+    <t>Q1_2023_Expenditures__c</t>
   </si>
   <si>
-    <t>Version: 2022.12.13</t>
+    <t>Version: 2023.4.18</t>
   </si>
 </sst>
 </file>
@@ -35185,21 +35185,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35416,32 +35401,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35458,4 +35433,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: update q1 2023 output templates (#1273) (#1274)
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 4 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pridgenc\Downloads\SLFRFBulkUploadTemplates\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C15497B-6C8E-434C-9B6A-CDFB32373EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16356CFA-53BD-4FBD-B03E-C69286943FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="4845" windowWidth="25815" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Q4_2022_Obligations__c</t>
+    <t>Q1_2023_Obligations__c</t>
   </si>
   <si>
-    <t>Q4_2022_Expenditures__c</t>
+    <t>Q1_2023_Expenditures__c</t>
   </si>
   <si>
-    <t>Version: 2022.12.13</t>
+    <t>Version: 2023.4.18</t>
   </si>
 </sst>
 </file>
@@ -35185,21 +35185,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35416,32 +35401,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35458,4 +35433,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Prod Release April 23 (#1276)
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 4 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pridgenc\Downloads\SLFRFBulkUploadTemplates\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C15497B-6C8E-434C-9B6A-CDFB32373EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16356CFA-53BD-4FBD-B03E-C69286943FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="4845" windowWidth="25815" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Q4_2022_Obligations__c</t>
+    <t>Q1_2023_Obligations__c</t>
   </si>
   <si>
-    <t>Q4_2022_Expenditures__c</t>
+    <t>Q1_2023_Expenditures__c</t>
   </si>
   <si>
-    <t>Version: 2022.12.13</t>
+    <t>Version: 2023.4.18</t>
   </si>
 </sst>
 </file>
@@ -35185,21 +35185,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35416,32 +35401,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35458,4 +35433,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit the latest version of treasury's bulk upload templates
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pridgenc\Downloads\SLFRFBulkUploadTemplates\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 2 2023 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16356CFA-53BD-4FBD-B03E-C69286943FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C421ABD9-0D04-4F6A-BFC7-91E80AFC4231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="4845" windowWidth="25815" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37620" yWindow="-4455" windowWidth="27420" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Q1_2023_Obligations__c</t>
+    <t>Version: 2023.5.17</t>
   </si>
   <si>
-    <t>Q1_2023_Expenditures__c</t>
+    <t>Q2_2023_Obligations__c</t>
   </si>
   <si>
-    <t>Version: 2023.4.18</t>
+    <t>Q2_2023_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FAA55-771D-4D64-A81A-E1231934DFE3}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -923,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1061,10 +1063,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>30</v>
@@ -35185,6 +35187,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35401,15 +35412,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -35417,6 +35419,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35431,14 +35441,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Commit the latest version of treasury's bulk upload templates (#1787)
* Commit the latest version of treasury's bulk upload templates

* Run: yarn parse-output-templates
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pridgenc\Downloads\SLFRFBulkUploadTemplates\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 2 2023 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16356CFA-53BD-4FBD-B03E-C69286943FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C421ABD9-0D04-4F6A-BFC7-91E80AFC4231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="4845" windowWidth="25815" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37620" yWindow="-4455" windowWidth="27420" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Q1_2023_Obligations__c</t>
+    <t>Version: 2023.5.17</t>
   </si>
   <si>
-    <t>Q1_2023_Expenditures__c</t>
+    <t>Q2_2023_Obligations__c</t>
   </si>
   <si>
-    <t>Version: 2023.4.18</t>
+    <t>Q2_2023_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FAA55-771D-4D64-A81A-E1231934DFE3}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -923,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1061,10 +1063,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>30</v>
@@ -35185,6 +35187,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35401,15 +35412,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -35417,6 +35419,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35431,14 +35441,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Commit the latest version of treasury's bulk upload templates (#1787) (#1883)
* feat(1303): add capital expenditure amount column to new project summary sheets (#1696)

Add column for capital expenditure amount in new project summary sheet and fix calculation for columns.

* Add datadog spans for file I/O and XLSX parsing (#1732)

* Add datadog span traces to file I/O and XLSX parsing

* Add tracing spans to workbook write operations

* Fix typo: tracer.tracer -> tracer.trace (#1785)

* Commit the latest version of treasury's bulk upload templates (#1787)

* Commit the latest version of treasury's bulk upload templates

* Run: yarn parse-output-templates

---------

Co-authored-by: michelle <mlam8428@gmail.com>
Co-authored-by: aditya <asridhar@usdigitalresponse.org>
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pridgenc\Downloads\SLFRFBulkUploadTemplates\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\Quarter 2 2023 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16356CFA-53BD-4FBD-B03E-C69286943FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C421ABD9-0D04-4F6A-BFC7-91E80AFC4231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="4845" windowWidth="25815" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37620" yWindow="-4455" windowWidth="27420" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -450,13 +450,13 @@
 (Text - max character 255)</t>
   </si>
   <si>
-    <t>Q1_2023_Obligations__c</t>
+    <t>Version: 2023.5.17</t>
   </si>
   <si>
-    <t>Q1_2023_Expenditures__c</t>
+    <t>Q2_2023_Obligations__c</t>
   </si>
   <si>
-    <t>Version: 2023.4.18</t>
+    <t>Q2_2023_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FAA55-771D-4D64-A81A-E1231934DFE3}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -923,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1061,10 +1063,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>30</v>
@@ -35185,6 +35187,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -35401,15 +35412,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -35417,6 +35419,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35431,14 +35441,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
chore: update export templates (v2024-07) (#3226)
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Downloads\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 1 2024 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Downloads\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 2 2024 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6CEFED-434B-4D96-AB7A-CB8F19D9B5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A4BD4C-68FB-4906-AFA5-22B78F4B3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,12 +453,6 @@
     <t>Version: 2023.5.17</t>
   </si>
   <si>
-    <t>Q1_2024_Obligations__c</t>
-  </si>
-  <si>
-    <t>Q1_2024_Expenditures__c</t>
-  </si>
-  <si>
     <t>Project_Start_Date__c</t>
   </si>
   <si>
@@ -479,6 +473,12 @@
     <t>REQUIRED if the project has completed. 
 REQUIRED if you selected "Completed" for the "Status to Completion" question. 
 End date  Valid Date - (MM/DD/YYYY)</t>
+  </si>
+  <si>
+    <t>Q2_2024_Obligations__c</t>
+  </si>
+  <si>
+    <t>Q2_2024_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -1082,10 +1082,10 @@
         <v>88</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>6</v>
@@ -1097,10 +1097,10 @@
         <v>8</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>30</v>
@@ -1286,10 +1286,10 @@
         <v>89</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>14</v>
@@ -1388,10 +1388,10 @@
         <v>91</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>86</v>
@@ -37223,15 +37223,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -37448,6 +37439,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -37455,14 +37455,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37477,6 +37469,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
chore: update to using the lastest treasury templates from 10_1_2024
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Downloads\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 2 2024 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd93f4fa04466af4/Desktop/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/Quarter 3 2024 Project Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A4BD4C-68FB-4906-AFA5-22B78F4B3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{74A4BD4C-68FB-4906-AFA5-22B78F4B3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A32843F2-B9F5-4E4C-8F27-335856C22A6D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,10 +475,10 @@
 End date  Valid Date - (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Q2_2024_Obligations__c</t>
+    <t>Q3_2024_Obligations__c</t>
   </si>
   <si>
-    <t>Q2_2024_Expenditures__c</t>
+    <t>Q3_2024_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:AH1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37223,6 +37223,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -37439,22 +37454,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37471,29 +37496,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update output file version to 2024-10-01 (#3563)
* chore: update to using the lastest treasury templates from 10_1_2024

* chore: run script to parse out file differences from previous quarter to current workbook
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Downloads\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 2 2024 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd93f4fa04466af4/Desktop/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/Quarter 3 2024 Project Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A4BD4C-68FB-4906-AFA5-22B78F4B3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{74A4BD4C-68FB-4906-AFA5-22B78F4B3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A32843F2-B9F5-4E4C-8F27-335856C22A6D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,10 +475,10 @@
 End date  Valid Date - (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Q2_2024_Obligations__c</t>
+    <t>Q3_2024_Obligations__c</t>
   </si>
   <si>
-    <t>Q2_2024_Expenditures__c</t>
+    <t>Q3_2024_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:AH1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37223,6 +37223,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -37439,22 +37454,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37471,29 +37496,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore: add new q4-2024 files
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd93f4fa04466af4/Desktop/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/Quarter 3 2024 Project Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Downloads\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 4 2024 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{74A4BD4C-68FB-4906-AFA5-22B78F4B3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A32843F2-B9F5-4E4C-8F27-335856C22A6D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D0E71B-572D-4458-908C-6EE36A4E507D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,10 +475,10 @@
 End date  Valid Date - (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Q3_2024_Obligations__c</t>
+    <t>Q4_2024_Obligations__c</t>
   </si>
   <si>
-    <t>Q3_2024_Expenditures__c</t>
+    <t>Q4_2024_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:AH1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37223,21 +37223,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -37454,32 +37439,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37496,4 +37471,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chore - Update output templates for Q4-2024 (#3845)
* chore: add new q4-2024 files

* chore: update output-template
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd93f4fa04466af4/Desktop/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/Quarter 3 2024 Project Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Downloads\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 4 2024 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{74A4BD4C-68FB-4906-AFA5-22B78F4B3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A32843F2-B9F5-4E4C-8F27-335856C22A6D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D0E71B-572D-4458-908C-6EE36A4E507D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,10 +475,10 @@
 End date  Valid Date - (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Q3_2024_Obligations__c</t>
+    <t>Q4_2024_Obligations__c</t>
   </si>
   <si>
-    <t>Q3_2024_Expenditures__c</t>
+    <t>Q4_2024_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:AH1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37223,21 +37223,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -37454,32 +37439,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37496,4 +37471,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>